<commit_message>
Changes Made: -FIX TIN and etc window showing up when in inventory mode -Inventory Mode is closed when the user has finished using it. Next Up: -Need to get rid of 100 divisor for Discount as it is already the right decimal value -Change "Cost" header to "Amount" for header label in app -Change Variables in TIN window to just be blank (i.e. one space) instead of "N/A" -Change "Item Number" to "Bar Code" inside word doc generation -Block "Proceed" button during purchase details window when change is less than 0 -Change Excel generation to include cost breakdown of items, create Cash, Debit, Credit, Check, Salary Deduction columns -Change Colors of program (Plain Color) -Figure our printing function -Add commas to separate thousands' vaulue when printing receipt -Make sure prices are in two decimal places -Align VAT Tax values -*EXTRA* Change line generation from right to left instead of left to right
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Final Product List" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Final Product List" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Final Product List'!$A$4:$E$238</definedName>
@@ -772,7 +772,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="25">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -800,140 +800,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <sz val="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <sz val="10"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -949,175 +816,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="31"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="46"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="36"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="52"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.7999816888943144"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.3999755851924192"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1140,245 +847,55 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.3999755851924192"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="45">
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="5" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="9" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="10" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="11" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="12" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="6" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="13" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="14" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="15" fontId="6" numFmtId="0"/>
-    <xf borderId="0" fillId="16" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="17" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="6" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="7" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="18" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="8" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="19" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="20" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="21" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="22" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="23" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="24" fontId="7" numFmtId="0"/>
-    <xf borderId="0" fillId="25" fontId="8" numFmtId="0"/>
-    <xf borderId="2" fillId="26" fontId="9" numFmtId="0"/>
-    <xf borderId="3" fillId="27" fontId="10" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0"/>
-    <xf borderId="0" fillId="28" fontId="12" numFmtId="0"/>
-    <xf borderId="4" fillId="0" fontId="13" numFmtId="0"/>
-    <xf borderId="5" fillId="0" fontId="14" numFmtId="0"/>
-    <xf borderId="6" fillId="0" fontId="15" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0"/>
-    <xf borderId="2" fillId="29" fontId="16" numFmtId="0"/>
-    <xf borderId="7" fillId="0" fontId="17" numFmtId="0"/>
-    <xf borderId="0" fillId="30" fontId="18" numFmtId="0"/>
+  <cellStyleXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="8" fillId="31" fontId="1" numFmtId="0"/>
-    <xf borderId="9" fillId="26" fontId="19" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0"/>
-    <xf borderId="10" fillId="0" fontId="21" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="37"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="37"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="23" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="23" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="23" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="5" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="24" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="37">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="4" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="24" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="40">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="9" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="24" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="37"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="4">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="30" name="20% - Accent1" xfId="1"/>
-    <cellStyle builtinId="34" name="20% - Accent2" xfId="2"/>
-    <cellStyle builtinId="38" name="20% - Accent3" xfId="3"/>
-    <cellStyle builtinId="42" name="20% - Accent4" xfId="4"/>
-    <cellStyle builtinId="46" name="20% - Accent5" xfId="5"/>
-    <cellStyle builtinId="50" name="20% - Accent6" xfId="6"/>
-    <cellStyle builtinId="31" name="40% - Accent1" xfId="7"/>
-    <cellStyle builtinId="35" name="40% - Accent2" xfId="8"/>
-    <cellStyle builtinId="39" name="40% - Accent3" xfId="9"/>
-    <cellStyle builtinId="43" name="40% - Accent4" xfId="10"/>
-    <cellStyle builtinId="47" name="40% - Accent5" xfId="11"/>
-    <cellStyle builtinId="51" name="40% - Accent6" xfId="12"/>
-    <cellStyle builtinId="32" name="60% - Accent1" xfId="13"/>
-    <cellStyle builtinId="36" name="60% - Accent2" xfId="14"/>
-    <cellStyle builtinId="40" name="60% - Accent3" xfId="15"/>
-    <cellStyle builtinId="44" name="60% - Accent4" xfId="16"/>
-    <cellStyle builtinId="48" name="60% - Accent5" xfId="17"/>
-    <cellStyle builtinId="52" name="60% - Accent6" xfId="18"/>
-    <cellStyle builtinId="29" name="Accent1" xfId="19"/>
-    <cellStyle builtinId="33" name="Accent2" xfId="20"/>
-    <cellStyle builtinId="37" name="Accent3" xfId="21"/>
-    <cellStyle builtinId="41" name="Accent4" xfId="22"/>
-    <cellStyle builtinId="45" name="Accent5" xfId="23"/>
-    <cellStyle builtinId="49" name="Accent6" xfId="24"/>
-    <cellStyle builtinId="27" name="Bad" xfId="25"/>
-    <cellStyle builtinId="22" name="Calculation" xfId="26"/>
-    <cellStyle builtinId="23" name="Check Cell" xfId="27"/>
-    <cellStyle builtinId="53" name="Explanatory Text" xfId="28"/>
-    <cellStyle builtinId="26" name="Good" xfId="29"/>
-    <cellStyle builtinId="16" name="Heading 1" xfId="30"/>
-    <cellStyle builtinId="17" name="Heading 2" xfId="31"/>
-    <cellStyle builtinId="18" name="Heading 3" xfId="32"/>
-    <cellStyle builtinId="19" name="Heading 4" xfId="33"/>
-    <cellStyle builtinId="20" name="Input" xfId="34"/>
-    <cellStyle builtinId="24" name="Linked Cell" xfId="35"/>
-    <cellStyle builtinId="28" name="Neutral" xfId="36"/>
-    <cellStyle name="Normal 2" xfId="37"/>
-    <cellStyle builtinId="10" name="Note" xfId="38"/>
-    <cellStyle builtinId="21" name="Output" xfId="39"/>
-    <cellStyle builtinId="5" name="Percent" xfId="40"/>
-    <cellStyle name="Percent 2" xfId="41"/>
-    <cellStyle builtinId="15" name="Title" xfId="42"/>
-    <cellStyle builtinId="25" name="Total" xfId="43"/>
-    <cellStyle builtinId="11" name="Warning Text" xfId="44"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle name="Percent 2" xfId="3"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -1715,7 +1232,7 @@
       <pane activePane="bottomRight" state="frozen" topLeftCell="C5" xSplit="2" ySplit="4"/>
       <selection activeCell="C1" pane="topRight" sqref="C1"/>
       <selection activeCell="A5" pane="bottomLeft" sqref="A5"/>
-      <selection activeCell="J2" pane="bottomRight" sqref="J2"/>
+      <selection activeCell="D5" pane="bottomRight" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.109375" defaultRowHeight="13.2" outlineLevelCol="0"/>
@@ -1725,16 +1242,17 @@
     <col bestFit="1" customWidth="1" max="3" min="3" style="4" width="14"/>
     <col bestFit="1" customWidth="1" max="4" min="4" style="5" width="10.6640625"/>
     <col bestFit="1" customWidth="1" max="5" min="5" style="6" width="18"/>
-    <col customWidth="1" max="16384" min="6" style="3" width="9.109375"/>
+    <col customWidth="1" max="6" min="6" style="3" width="9.109375"/>
+    <col customWidth="1" max="16384" min="7" style="3" width="9.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row customHeight="1" ht="14.4" r="1" spans="1:6">
       <c r="F1" t="s"/>
     </row>
-    <row r="2" spans="1:6">
+    <row customHeight="1" ht="14.4" r="2" spans="1:6">
       <c r="F2" t="s"/>
     </row>
-    <row r="3" spans="1:6">
+    <row customHeight="1" ht="14.4" r="3" spans="1:6">
       <c r="F3" t="s"/>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="4" s="2" spans="1:6">
@@ -1758,30 +1276,30 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="5" s="1" spans="1:6">
-      <c r="A5" s="14" t="n">
+      <c r="A5" s="13" t="n">
         <v>20297939</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="10" t="n">
         <v>250</v>
       </c>
       <c r="D5" s="11" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E5" s="12" t="n">
         <v>3605520297939</v>
       </c>
       <c r="F5" s="12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="6" s="1" spans="1:6">
-      <c r="A6" s="14" t="n">
+      <c r="A6" s="13" t="n">
         <v>72728313</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="10" t="n">
@@ -1798,10 +1316,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="7" s="1" spans="1:6">
-      <c r="A7" s="14" t="n">
+      <c r="A7" s="13" t="n">
         <v>20267093</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10" t="n">
@@ -1818,10 +1336,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="8" s="1" spans="1:6">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="13" t="n">
         <v>20297878</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="10" t="n">
@@ -1838,10 +1356,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="9" s="1" spans="1:6">
-      <c r="A9" s="14" t="n">
+      <c r="A9" s="13" t="n">
         <v>70638152</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="10" t="n">
@@ -1858,10 +1376,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="10" s="1" spans="1:6">
-      <c r="A10" s="14" t="n">
+      <c r="A10" s="13" t="n">
         <v>71381477</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="10" t="n">
@@ -1878,10 +1396,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="11" s="1" spans="1:6">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="13" t="n">
         <v>71381538</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="10" t="n">
@@ -1898,10 +1416,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="12" s="1" spans="1:6">
-      <c r="A12" s="14" t="n">
+      <c r="A12" s="13" t="n">
         <v>71381392</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="10" t="n">
@@ -1918,10 +1436,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="13" s="1" spans="1:6">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="13" t="n">
         <v>71381491</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="10" t="n">
@@ -1938,10 +1456,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="14" s="1" spans="1:6">
-      <c r="A14" s="14" t="n">
+      <c r="A14" s="13" t="n">
         <v>70157639</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="10" t="n">
@@ -1958,10 +1476,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="15" s="1" spans="1:6">
-      <c r="A15" s="14" t="n">
+      <c r="A15" s="13" t="n">
         <v>22035423</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="10" t="n">
@@ -1978,10 +1496,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="16" s="1" spans="1:6">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="13" t="n">
         <v>71214799</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="10" t="n">
@@ -1998,10 +1516,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="17" s="1" spans="1:6">
-      <c r="A17" s="14" t="n">
+      <c r="A17" s="13" t="n">
         <v>21583413</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="10" t="n">
@@ -2018,10 +1536,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="18" s="1" spans="1:6">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="13" t="n">
         <v>72009436</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="10" t="n">
@@ -2038,10 +1556,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="19" s="1" spans="1:6">
-      <c r="A19" s="14" t="n">
+      <c r="A19" s="13" t="n">
         <v>30655201</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>20</v>
       </c>
       <c r="C19" s="10" t="n">
@@ -2058,10 +1576,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="20" s="1" spans="1:6">
-      <c r="A20" s="14" t="n">
+      <c r="A20" s="13" t="n">
         <v>30543003</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="10" t="n">
@@ -2078,10 +1596,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="21" s="1" spans="1:6">
-      <c r="A21" s="14" t="n">
+      <c r="A21" s="13" t="n">
         <v>30542709</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C21" s="10" t="n">
@@ -2098,10 +1616,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="22" s="1" spans="1:6">
-      <c r="A22" s="14" t="n">
+      <c r="A22" s="13" t="n">
         <v>36382378</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="10" t="n">
@@ -2118,10 +1636,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="23" s="1" spans="1:6">
-      <c r="A23" s="14" t="n">
+      <c r="A23" s="13" t="n">
         <v>36382361</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="10" t="n">
@@ -2138,10 +1656,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="24" s="1" spans="1:6">
-      <c r="A24" s="14" t="n">
+      <c r="A24" s="13" t="n">
         <v>36471751</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="10" t="n">
@@ -2158,10 +1676,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="25" s="1" spans="1:6">
-      <c r="A25" s="14" t="n">
+      <c r="A25" s="13" t="n">
         <v>36218684</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="10" t="n">
@@ -2178,10 +1696,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="26" s="1" spans="1:6">
-      <c r="A26" s="14" t="n">
+      <c r="A26" s="13" t="n">
         <v>36218745</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="10" t="n">
@@ -2198,10 +1716,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="27" s="1" spans="1:6">
-      <c r="A27" s="14" t="n">
+      <c r="A27" s="13" t="n">
         <v>30647374</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="10" t="n">
@@ -2218,10 +1736,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="28" s="1" spans="1:6">
-      <c r="A28" s="14" t="n">
+      <c r="A28" s="13" t="n">
         <v>30713383</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="10" t="n">
@@ -2238,10 +1756,10 @@
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="14.4" r="29" s="1" spans="1:6">
-      <c r="A29" s="14" t="n">
+      <c r="A29" s="13" t="n">
         <v>36382736</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="10" t="n">
@@ -2258,10 +1776,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="30" spans="1:6">
-      <c r="A30" s="14" t="n">
+      <c r="A30" s="13" t="n">
         <v>36398867</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="10" t="n">
@@ -2278,10 +1796,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="31" spans="1:6">
-      <c r="A31" s="14" t="n">
+      <c r="A31" s="13" t="n">
         <v>36397402</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="10" t="n">
@@ -2298,10 +1816,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="32" spans="1:6">
-      <c r="A32" s="14" t="n">
+      <c r="A32" s="13" t="n">
         <v>36382682</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="10" t="n">
@@ -2318,10 +1836,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="33" spans="1:6">
-      <c r="A33" s="14" t="n">
+      <c r="A33" s="13" t="n">
         <v>36403912</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="10" t="n">
@@ -2338,10 +1856,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="34" spans="1:6">
-      <c r="A34" s="14" t="n">
+      <c r="A34" s="13" t="n">
         <v>36356065</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="10" t="n">
@@ -2358,10 +1876,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="35" spans="1:6">
-      <c r="A35" s="14" t="n">
+      <c r="A35" s="13" t="n">
         <v>36494767</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="10" t="n">
@@ -2378,10 +1896,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="36" spans="1:6">
-      <c r="A36" s="14" t="n">
+      <c r="A36" s="13" t="n">
         <v>36397532</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="10" t="n">
@@ -2398,10 +1916,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="37" spans="1:6">
-      <c r="A37" s="14" t="n">
+      <c r="A37" s="13" t="n">
         <v>36397556</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="10" t="n">
@@ -2418,10 +1936,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="38" spans="1:6">
-      <c r="A38" s="14" t="n">
+      <c r="A38" s="13" t="n">
         <v>36400232</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C38" s="10" t="n">
@@ -2438,10 +1956,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="39" spans="1:6">
-      <c r="A39" s="14" t="n">
+      <c r="A39" s="13" t="n">
         <v>36398850</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="10" t="n">
@@ -2458,10 +1976,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="40" spans="1:6">
-      <c r="A40" s="14" t="n">
+      <c r="A40" s="13" t="n">
         <v>36382668</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C40" s="10" t="n">
@@ -2478,10 +1996,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="41" spans="1:6">
-      <c r="A41" s="14" t="n">
+      <c r="A41" s="13" t="n">
         <v>36397952</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="10" t="n">
@@ -2498,10 +2016,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="42" spans="1:6">
-      <c r="A42" s="14" t="n">
+      <c r="A42" s="13" t="n">
         <v>36494859</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C42" s="10" t="n">
@@ -2518,10 +2036,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="43" spans="1:6">
-      <c r="A43" s="14" t="n">
+      <c r="A43" s="13" t="n">
         <v>36397983</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>44</v>
       </c>
       <c r="C43" s="10" t="n">
@@ -2538,10 +2056,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="44" spans="1:6">
-      <c r="A44" s="14" t="n">
+      <c r="A44" s="13" t="n">
         <v>36398850</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C44" s="10" t="n">
@@ -2558,10 +2076,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="45" spans="1:6">
-      <c r="A45" s="14" t="n">
+      <c r="A45" s="13" t="n">
         <v>36382705</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C45" s="10" t="n">
@@ -2578,10 +2096,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="46" spans="1:6">
-      <c r="A46" s="14" t="n">
+      <c r="A46" s="13" t="n">
         <v>36400218</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C46" s="10" t="n">
@@ -2598,10 +2116,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="47" spans="1:6">
-      <c r="A47" s="14" t="n">
+      <c r="A47" s="13" t="n">
         <v>36400201</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="13" t="s">
         <v>47</v>
       </c>
       <c r="C47" s="10" t="n">
@@ -2618,10 +2136,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="48" spans="1:6">
-      <c r="A48" s="14" t="n">
+      <c r="A48" s="13" t="n">
         <v>30152540</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C48" s="10" t="n">
@@ -2638,10 +2156,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="49" spans="1:6">
-      <c r="A49" s="14" t="n">
+      <c r="A49" s="13" t="n">
         <v>30458222</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>49</v>
       </c>
       <c r="C49" s="10" t="n">
@@ -2658,10 +2176,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="50" spans="1:6">
-      <c r="A50" s="14" t="n">
+      <c r="A50" s="13" t="n">
         <v>30457621</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>50</v>
       </c>
       <c r="C50" s="10" t="n">
@@ -2678,10 +2196,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="51" spans="1:6">
-      <c r="A51" s="14" t="n">
+      <c r="A51" s="13" t="n">
         <v>30458062</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>51</v>
       </c>
       <c r="C51" s="10" t="n">
@@ -2698,10 +2216,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="52" spans="1:6">
-      <c r="A52" s="14" t="n">
+      <c r="A52" s="13" t="n">
         <v>36356003</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C52" s="10" t="n">
@@ -2718,10 +2236,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="53" spans="1:6">
-      <c r="A53" s="14" t="n">
+      <c r="A53" s="13" t="n">
         <v>30530836</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="13" t="s">
         <v>53</v>
       </c>
       <c r="C53" s="10" t="n">
@@ -2738,10 +2256,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="54" spans="1:6">
-      <c r="A54" s="14" t="n">
+      <c r="A54" s="13" t="n">
         <v>36356003</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C54" s="10" t="n">
@@ -2758,10 +2276,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="55" spans="1:6">
-      <c r="A55" s="14" t="n">
+      <c r="A55" s="13" t="n">
         <v>30525658</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>54</v>
       </c>
       <c r="C55" s="10" t="n">
@@ -2778,10 +2296,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="56" spans="1:6">
-      <c r="A56" s="14" t="n">
+      <c r="A56" s="13" t="n">
         <v>26404810</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>55</v>
       </c>
       <c r="C56" s="10" t="n">
@@ -2798,10 +2316,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="57" spans="1:6">
-      <c r="A57" s="14" t="n">
+      <c r="A57" s="13" t="n">
         <v>30614727</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>56</v>
       </c>
       <c r="C57" s="10" t="n">
@@ -2818,10 +2336,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="58" spans="1:6">
-      <c r="A58" s="14" t="n">
+      <c r="A58" s="13" t="n">
         <v>30641044</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>57</v>
       </c>
       <c r="C58" s="10" t="n">
@@ -2838,10 +2356,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="59" spans="1:6">
-      <c r="A59" s="14" t="n">
+      <c r="A59" s="13" t="n">
         <v>30714762</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>58</v>
       </c>
       <c r="C59" s="10" t="n">
@@ -2858,10 +2376,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="60" spans="1:6">
-      <c r="A60" s="14" t="n">
+      <c r="A60" s="13" t="n">
         <v>30525870</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>59</v>
       </c>
       <c r="C60" s="10" t="n">
@@ -2878,10 +2396,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="61" spans="1:6">
-      <c r="A61" s="14" t="n">
+      <c r="A61" s="13" t="n">
         <v>30640702</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C61" s="10" t="n">
@@ -2898,10 +2416,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="62" spans="1:6">
-      <c r="A62" s="14" t="n">
+      <c r="A62" s="13" t="n">
         <v>30640702</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>60</v>
       </c>
       <c r="C62" s="10" t="n">
@@ -2918,10 +2436,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="63" spans="1:6">
-      <c r="A63" s="14" t="n">
+      <c r="A63" s="13" t="n">
         <v>30633698</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="13" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="10" t="n">
@@ -2938,10 +2456,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="64" spans="1:6">
-      <c r="A64" s="14" t="n">
+      <c r="A64" s="13" t="n">
         <v>30640504</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="13" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="10" t="n">
@@ -2958,10 +2476,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="65" spans="1:6">
-      <c r="A65" s="14" t="n">
+      <c r="A65" s="13" t="n">
         <v>30714946</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C65" s="10" t="n">
@@ -2978,10 +2496,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="66" spans="1:6">
-      <c r="A66" s="14" t="n">
+      <c r="A66" s="13" t="n">
         <v>30714946</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>63</v>
       </c>
       <c r="C66" s="10" t="n">
@@ -2998,10 +2516,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="67" spans="1:6">
-      <c r="A67" s="14" t="n">
+      <c r="A67" s="13" t="n">
         <v>36202430</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C67" s="10" t="n">
@@ -3018,10 +2536,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="68" spans="1:6">
-      <c r="A68" s="14" t="n">
+      <c r="A68" s="13" t="n">
         <v>30471764</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="13" t="s">
         <v>65</v>
       </c>
       <c r="C68" s="10" t="n">
@@ -3038,10 +2556,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="69" spans="1:6">
-      <c r="A69" s="14" t="n">
+      <c r="A69" s="13" t="n">
         <v>36202430</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="10" t="n">
@@ -3058,10 +2576,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="70" spans="1:6">
-      <c r="A70" s="14" t="n">
+      <c r="A70" s="13" t="n">
         <v>30536081</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C70" s="10" t="n">
@@ -3078,10 +2596,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="71" spans="1:6">
-      <c r="A71" s="14" t="n">
+      <c r="A71" s="13" t="n">
         <v>36391097</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="13" t="s">
         <v>67</v>
       </c>
       <c r="C71" s="10" t="n">
@@ -3098,10 +2616,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="72" spans="1:6">
-      <c r="A72" s="14" t="n">
+      <c r="A72" s="13" t="n">
         <v>30632196</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="13" t="s">
         <v>68</v>
       </c>
       <c r="C72" s="10" t="n">
@@ -3118,10 +2636,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="73" spans="1:6">
-      <c r="A73" s="14" t="n">
+      <c r="A73" s="13" t="n">
         <v>30698741</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C73" s="10" t="n">
@@ -3138,10 +2656,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="74" spans="1:6">
-      <c r="A74" s="14" t="n">
+      <c r="A74" s="13" t="n">
         <v>36501960</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C74" s="10" t="n">
@@ -3158,10 +2676,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="75" spans="1:6">
-      <c r="A75" s="14" t="n">
+      <c r="A75" s="13" t="n">
         <v>30643659</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C75" s="10" t="n">
@@ -3178,10 +2696,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="76" spans="1:6">
-      <c r="A76" s="14" t="n">
+      <c r="A76" s="13" t="n">
         <v>18250953</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C76" s="10" t="n">
@@ -3198,10 +2716,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="77" spans="1:6">
-      <c r="A77" s="15" t="n">
+      <c r="A77" s="14" t="n">
         <v>30633629</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C77" s="10" t="n">
@@ -3218,10 +2736,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="78" spans="1:6">
-      <c r="A78" s="15" t="n">
+      <c r="A78" s="14" t="n">
         <v>18251585</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C78" s="10" t="n">
@@ -3238,10 +2756,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="79" spans="1:6">
-      <c r="A79" s="15" t="n">
+      <c r="A79" s="14" t="n">
         <v>18250816</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C79" s="10" t="n">
@@ -3258,10 +2776,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="80" spans="1:6">
-      <c r="A80" s="15" t="n">
+      <c r="A80" s="14" t="n">
         <v>30262263</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C80" s="10" t="n">
@@ -3278,10 +2796,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="81" spans="1:6">
-      <c r="A81" s="15" t="n">
+      <c r="A81" s="14" t="n">
         <v>32000481</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="13" t="s">
         <v>77</v>
       </c>
       <c r="C81" s="10" t="n">
@@ -3298,10 +2816,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="82" spans="1:6">
-      <c r="A82" s="15" t="n">
+      <c r="A82" s="14" t="n">
         <v>30643611</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="13" t="s">
         <v>78</v>
       </c>
       <c r="C82" s="10" t="n">
@@ -3318,10 +2836,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="83" spans="1:6">
-      <c r="A83" s="15" t="n">
+      <c r="A83" s="14" t="n">
         <v>30640825</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="13" t="s">
         <v>79</v>
       </c>
       <c r="C83" s="10" t="n">
@@ -3338,10 +2856,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="84" spans="1:6">
-      <c r="A84" s="15" t="n">
+      <c r="A84" s="14" t="n">
         <v>30714649</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="13" t="s">
         <v>80</v>
       </c>
       <c r="C84" s="10" t="n">
@@ -3358,10 +2876,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="85" spans="1:6">
-      <c r="A85" s="15" t="n">
+      <c r="A85" s="14" t="n">
         <v>22895844</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="13" t="s">
         <v>81</v>
       </c>
       <c r="C85" s="10" t="n">
@@ -3378,10 +2896,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="86" spans="1:6">
-      <c r="A86" s="15" t="n">
+      <c r="A86" s="14" t="n">
         <v>18251615</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C86" s="10" t="n">
@@ -3398,10 +2916,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="87" spans="1:6">
-      <c r="A87" s="15" t="n">
+      <c r="A87" s="14" t="n">
         <v>18251615</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C87" s="10" t="n">
@@ -3418,10 +2936,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="88" spans="1:6">
-      <c r="A88" s="15" t="n">
+      <c r="A88" s="14" t="n">
         <v>30643499</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C88" s="10" t="n">
@@ -3438,10 +2956,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="89" spans="1:6">
-      <c r="A89" s="15" t="n">
+      <c r="A89" s="14" t="n">
         <v>30643536</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="13" t="s">
         <v>84</v>
       </c>
       <c r="C89" s="10" t="n">
@@ -3458,10 +2976,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="90" spans="1:6">
-      <c r="A90" s="15" t="n">
+      <c r="A90" s="14" t="n">
         <v>22895714</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C90" s="10" t="n">
@@ -3478,10 +2996,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="91" spans="1:6">
-      <c r="A91" s="15" t="n">
+      <c r="A91" s="14" t="n">
         <v>36459438</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="13" t="s">
         <v>86</v>
       </c>
       <c r="C91" s="10" t="n">
@@ -3498,10 +3016,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="92" spans="1:6">
-      <c r="A92" s="15" t="n">
+      <c r="A92" s="14" t="n">
         <v>22895707</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="13" t="s">
         <v>87</v>
       </c>
       <c r="C92" s="10" t="n">
@@ -3518,10 +3036,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="93" spans="1:6">
-      <c r="A93" s="15" t="n">
+      <c r="A93" s="14" t="n">
         <v>86130594</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C93" s="10" t="n">
@@ -3538,10 +3056,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="94" spans="1:6">
-      <c r="A94" s="15" t="n">
+      <c r="A94" s="14" t="n">
         <v>86194183</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="13" t="s">
         <v>89</v>
       </c>
       <c r="C94" s="10" t="n">
@@ -3558,10 +3076,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="95" spans="1:6">
-      <c r="A95" s="15" t="n">
+      <c r="A95" s="14" t="n">
         <v>86194121</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="13" t="s">
         <v>90</v>
       </c>
       <c r="C95" s="10" t="n">
@@ -3578,10 +3096,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="96" spans="1:6">
-      <c r="A96" s="15" t="n">
+      <c r="A96" s="14" t="n">
         <v>86151377</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="13" t="s">
         <v>91</v>
       </c>
       <c r="C96" s="10" t="n">
@@ -3598,10 +3116,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="97" spans="1:6">
-      <c r="A97" s="15" t="n">
+      <c r="A97" s="14" t="n">
         <v>86152091</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="13" t="s">
         <v>92</v>
       </c>
       <c r="C97" s="10" t="n">
@@ -3618,10 +3136,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="98" spans="1:6">
-      <c r="A98" s="15" t="n">
+      <c r="A98" s="14" t="n">
         <v>86151889</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C98" s="10" t="n">
@@ -3638,10 +3156,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="99" spans="1:6">
-      <c r="A99" s="15" t="n">
+      <c r="A99" s="14" t="n">
         <v>86194206</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C99" s="10" t="n">
@@ -3658,10 +3176,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="100" spans="1:6">
-      <c r="A100" s="15" t="n">
+      <c r="A100" s="14" t="n">
         <v>86151612</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C100" s="10" t="n">
@@ -3678,10 +3196,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="101" spans="1:6">
-      <c r="A101" s="15" t="n">
+      <c r="A101" s="14" t="n">
         <v>18232867</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="13" t="s">
         <v>96</v>
       </c>
       <c r="C101" s="10" t="n">
@@ -3698,10 +3216,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="102" spans="1:6">
-      <c r="A102" s="15" t="n">
+      <c r="A102" s="14" t="n">
         <v>86151827</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="13" t="s">
         <v>97</v>
       </c>
       <c r="C102" s="10" t="n">
@@ -3718,10 +3236,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="103" spans="1:6">
-      <c r="A103" s="15" t="n">
+      <c r="A103" s="14" t="n">
         <v>86151513</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="13" t="s">
         <v>98</v>
       </c>
       <c r="C103" s="10" t="n">
@@ -3738,10 +3256,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="104" spans="1:6">
-      <c r="A104" s="15" t="n">
+      <c r="A104" s="14" t="n">
         <v>86152077</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="13" t="s">
         <v>99</v>
       </c>
       <c r="C104" s="10" t="n">
@@ -3758,10 +3276,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="105" spans="1:6">
-      <c r="A105" s="15" t="n">
+      <c r="A105" s="14" t="n">
         <v>86151315</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="13" t="s">
         <v>100</v>
       </c>
       <c r="C105" s="10" t="n">
@@ -3778,10 +3296,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="106" spans="1:6">
-      <c r="A106" s="15" t="n">
+      <c r="A106" s="14" t="n">
         <v>26407163</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="13" t="s">
         <v>101</v>
       </c>
       <c r="C106" s="10" t="n">
@@ -3798,10 +3316,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="107" spans="1:6">
-      <c r="A107" s="15" t="n">
+      <c r="A107" s="14" t="n">
         <v>30620421</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="13" t="s">
         <v>102</v>
       </c>
       <c r="C107" s="10" t="n">
@@ -3818,10 +3336,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="108" spans="1:6">
-      <c r="A108" s="15" t="n">
+      <c r="A108" s="14" t="n">
         <v>30620261</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="13" t="s">
         <v>103</v>
       </c>
       <c r="C108" s="10" t="n">
@@ -3838,10 +3356,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="109" spans="1:6">
-      <c r="A109" s="15" t="n">
+      <c r="A109" s="14" t="n">
         <v>18290263</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="13" t="s">
         <v>104</v>
       </c>
       <c r="C109" s="10" t="n">
@@ -3858,10 +3376,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="110" spans="1:6">
-      <c r="A110" s="15" t="n">
+      <c r="A110" s="14" t="n">
         <v>30620308</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B110" s="13" t="s">
         <v>105</v>
       </c>
       <c r="C110" s="10" t="n">
@@ -3878,10 +3396,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="111" spans="1:6">
-      <c r="A111" s="15" t="n">
+      <c r="A111" s="14" t="n">
         <v>30671942</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B111" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C111" s="10" t="n">
@@ -3898,10 +3416,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="112" spans="1:6">
-      <c r="A112" s="15" t="n">
+      <c r="A112" s="14" t="n">
         <v>26980987</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="13" t="s">
         <v>107</v>
       </c>
       <c r="C112" s="10" t="n">
@@ -3918,10 +3436,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="113" spans="1:6">
-      <c r="A113" s="15" t="n">
+      <c r="A113" s="14" t="n">
         <v>86151421</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" s="13" t="s">
         <v>108</v>
       </c>
       <c r="C113" s="10" t="n">
@@ -3938,10 +3456,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="114" spans="1:6">
-      <c r="A114" s="15" t="n">
+      <c r="A114" s="14" t="n">
         <v>26406852</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B114" s="13" t="s">
         <v>109</v>
       </c>
       <c r="C114" s="10" t="n">
@@ -3958,10 +3476,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="115" spans="1:6">
-      <c r="A115" s="15" t="n">
+      <c r="A115" s="14" t="n">
         <v>86151742</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="B115" s="13" t="s">
         <v>110</v>
       </c>
       <c r="C115" s="10" t="n">
@@ -3978,10 +3496,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="116" spans="1:6">
-      <c r="A116" s="15" t="n">
+      <c r="A116" s="14" t="n">
         <v>86151940</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="B116" s="13" t="s">
         <v>111</v>
       </c>
       <c r="C116" s="10" t="n">
@@ -3998,10 +3516,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="117" spans="1:6">
-      <c r="A117" s="15" t="n">
+      <c r="A117" s="14" t="n">
         <v>70859336</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="13" t="s">
         <v>112</v>
       </c>
       <c r="C117" s="10" t="n">
@@ -4018,10 +3536,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="118" spans="1:6">
-      <c r="A118" s="15" t="n">
+      <c r="A118" s="14" t="n">
         <v>70278755</v>
       </c>
-      <c r="B118" s="14" t="s">
+      <c r="B118" s="13" t="s">
         <v>113</v>
       </c>
       <c r="C118" s="10" t="n">
@@ -4038,10 +3556,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="119" spans="1:6">
-      <c r="A119" s="15" t="n">
+      <c r="A119" s="14" t="n">
         <v>70416089</v>
       </c>
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="13" t="s">
         <v>114</v>
       </c>
       <c r="C119" s="10" t="n">
@@ -4058,10 +3576,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="120" spans="1:6">
-      <c r="A120" s="15" t="n">
+      <c r="A120" s="14" t="n">
         <v>75071962</v>
       </c>
-      <c r="B120" s="14" t="s">
+      <c r="B120" s="13" t="s">
         <v>115</v>
       </c>
       <c r="C120" s="10" t="n">
@@ -4078,10 +3596,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="121" spans="1:6">
-      <c r="A121" s="15" t="n">
+      <c r="A121" s="14" t="n">
         <v>77002951</v>
       </c>
-      <c r="B121" s="14" t="s">
+      <c r="B121" s="13" t="s">
         <v>116</v>
       </c>
       <c r="C121" s="10" t="n">
@@ -4098,10 +3616,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="122" spans="1:6">
-      <c r="A122" s="15" t="n">
+      <c r="A122" s="14" t="n">
         <v>77022911</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="B122" s="13" t="s">
         <v>117</v>
       </c>
       <c r="C122" s="10" t="n">
@@ -4118,10 +3636,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="123" spans="1:6">
-      <c r="A123" s="15" t="n">
+      <c r="A123" s="14" t="n">
         <v>77032750</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B123" s="13" t="s">
         <v>118</v>
       </c>
       <c r="C123" s="10" t="n">
@@ -4138,10 +3656,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="124" spans="1:6">
-      <c r="A124" s="15" t="n">
+      <c r="A124" s="14" t="n">
         <v>72055402</v>
       </c>
-      <c r="B124" s="14" t="s">
+      <c r="B124" s="13" t="s">
         <v>119</v>
       </c>
       <c r="C124" s="10" t="n">
@@ -4158,10 +3676,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="125" spans="1:6">
-      <c r="A125" s="15" t="n">
+      <c r="A125" s="14" t="n">
         <v>71068010</v>
       </c>
-      <c r="B125" s="14" t="s">
+      <c r="B125" s="13" t="s">
         <v>120</v>
       </c>
       <c r="C125" s="10" t="n">
@@ -4178,10 +3696,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="126" spans="1:6">
-      <c r="A126" s="15" t="n">
+      <c r="A126" s="14" t="n">
         <v>70852856</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="B126" s="13" t="s">
         <v>121</v>
       </c>
       <c r="C126" s="10" t="n">
@@ -4198,10 +3716,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="127" spans="1:6">
-      <c r="A127" s="15" t="n">
+      <c r="A127" s="14" t="n">
         <v>70416003</v>
       </c>
-      <c r="B127" s="14" t="s">
+      <c r="B127" s="13" t="s">
         <v>122</v>
       </c>
       <c r="C127" s="10" t="n">
@@ -4218,10 +3736,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="128" spans="1:6">
-      <c r="A128" s="15" t="n">
+      <c r="A128" s="14" t="n">
         <v>70265519</v>
       </c>
-      <c r="B128" s="14" t="s">
+      <c r="B128" s="13" t="s">
         <v>123</v>
       </c>
       <c r="C128" s="10" t="n">
@@ -4238,10 +3756,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="129" spans="1:6">
-      <c r="A129" s="15" t="n">
+      <c r="A129" s="14" t="n">
         <v>71121586</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="13" t="s">
         <v>124</v>
       </c>
       <c r="C129" s="10" t="n">
@@ -4258,10 +3776,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="130" spans="1:6">
-      <c r="A130" s="15" t="n">
+      <c r="A130" s="14" t="n">
         <v>70649272</v>
       </c>
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="13" t="s">
         <v>125</v>
       </c>
       <c r="C130" s="10" t="n">
@@ -4278,10 +3796,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="131" spans="1:6">
-      <c r="A131" s="15" t="n">
+      <c r="A131" s="14" t="n">
         <v>71068492</v>
       </c>
-      <c r="B131" s="14" t="s">
+      <c r="B131" s="13" t="s">
         <v>126</v>
       </c>
       <c r="C131" s="10" t="n">
@@ -4298,10 +3816,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="132" spans="1:6">
-      <c r="A132" s="15" t="n">
+      <c r="A132" s="14" t="n">
         <v>71256165</v>
       </c>
-      <c r="B132" s="14" t="s">
+      <c r="B132" s="13" t="s">
         <v>127</v>
       </c>
       <c r="C132" s="10" t="n">
@@ -4318,10 +3836,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="133" spans="1:6">
-      <c r="A133" s="15" t="n">
+      <c r="A133" s="14" t="n">
         <v>71369780</v>
       </c>
-      <c r="B133" s="14" t="s">
+      <c r="B133" s="13" t="s">
         <v>128</v>
       </c>
       <c r="C133" s="10" t="n">
@@ -4338,10 +3856,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="134" spans="1:6">
-      <c r="A134" s="15" t="n">
+      <c r="A134" s="14" t="n">
         <v>71369704</v>
       </c>
-      <c r="B134" s="14" t="s">
+      <c r="B134" s="13" t="s">
         <v>129</v>
       </c>
       <c r="C134" s="10" t="n">
@@ -4358,10 +3876,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="135" spans="1:6">
-      <c r="A135" s="15" t="n">
+      <c r="A135" s="14" t="n">
         <v>71369346</v>
       </c>
-      <c r="B135" s="14" t="s">
+      <c r="B135" s="13" t="s">
         <v>130</v>
       </c>
       <c r="C135" s="10" t="n">
@@ -4378,10 +3896,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="136" spans="1:6">
-      <c r="A136" s="15" t="n">
+      <c r="A136" s="14" t="n">
         <v>71259609</v>
       </c>
-      <c r="B136" s="14" t="s">
+      <c r="B136" s="13" t="s">
         <v>131</v>
       </c>
       <c r="C136" s="10" t="n">
@@ -4398,10 +3916,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="137" spans="1:6">
-      <c r="A137" s="15" t="n">
+      <c r="A137" s="14" t="n">
         <v>71267680</v>
       </c>
-      <c r="B137" s="14" t="s">
+      <c r="B137" s="13" t="s">
         <v>132</v>
       </c>
       <c r="C137" s="10" t="n">
@@ -4418,10 +3936,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="138" spans="1:6">
-      <c r="A138" s="15" t="n">
+      <c r="A138" s="14" t="n">
         <v>71369261</v>
       </c>
-      <c r="B138" s="14" t="s">
+      <c r="B138" s="13" t="s">
         <v>133</v>
       </c>
       <c r="C138" s="10" t="n">
@@ -4438,10 +3956,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="139" spans="1:6">
-      <c r="A139" s="15" t="n">
+      <c r="A139" s="14" t="n">
         <v>71371288</v>
       </c>
-      <c r="B139" s="14" t="s">
+      <c r="B139" s="13" t="s">
         <v>134</v>
       </c>
       <c r="C139" s="10" t="n">
@@ -4458,10 +3976,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="140" spans="1:6">
-      <c r="A140" s="15" t="n">
+      <c r="A140" s="14" t="n">
         <v>71171499</v>
       </c>
-      <c r="B140" s="14" t="s">
+      <c r="B140" s="13" t="s">
         <v>135</v>
       </c>
       <c r="C140" s="10" t="n">
@@ -4478,10 +3996,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="141" spans="1:6">
-      <c r="A141" s="15" t="n">
+      <c r="A141" s="14" t="n">
         <v>71370069</v>
       </c>
-      <c r="B141" s="14" t="s">
+      <c r="B141" s="13" t="s">
         <v>136</v>
       </c>
       <c r="C141" s="10" t="n">
@@ -4498,10 +4016,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="142" spans="1:6">
-      <c r="A142" s="15" t="n">
+      <c r="A142" s="14" t="n">
         <v>71045455</v>
       </c>
-      <c r="B142" s="14" t="s">
+      <c r="B142" s="13" t="s">
         <v>137</v>
       </c>
       <c r="C142" s="10" t="n">
@@ -4518,10 +4036,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="143" spans="1:6">
-      <c r="A143" s="15" t="n">
+      <c r="A143" s="14" t="n">
         <v>71255601</v>
       </c>
-      <c r="B143" s="14" t="s">
+      <c r="B143" s="13" t="s">
         <v>138</v>
       </c>
       <c r="C143" s="10" t="n">
@@ -4538,10 +4056,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="144" spans="1:6">
-      <c r="A144" s="15" t="n">
+      <c r="A144" s="14" t="n">
         <v>71253447</v>
       </c>
-      <c r="B144" s="14" t="s">
+      <c r="B144" s="13" t="s">
         <v>139</v>
       </c>
       <c r="C144" s="10" t="n">
@@ -4558,10 +4076,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="145" spans="1:6">
-      <c r="A145" s="15" t="n">
+      <c r="A145" s="14" t="n">
         <v>71045738</v>
       </c>
-      <c r="B145" s="14" t="s">
+      <c r="B145" s="13" t="s">
         <v>140</v>
       </c>
       <c r="C145" s="10" t="n">
@@ -4578,10 +4096,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="146" spans="1:6">
-      <c r="A146" s="15" t="n">
+      <c r="A146" s="14" t="n">
         <v>71235962</v>
       </c>
-      <c r="B146" s="14" t="s">
+      <c r="B146" s="13" t="s">
         <v>141</v>
       </c>
       <c r="C146" s="10" t="n">
@@ -4598,10 +4116,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="147" spans="1:6">
-      <c r="A147" s="15" t="n">
+      <c r="A147" s="14" t="n">
         <v>71168772</v>
       </c>
-      <c r="B147" s="14" t="s">
+      <c r="B147" s="13" t="s">
         <v>142</v>
       </c>
       <c r="C147" s="10" t="n">
@@ -4618,10 +4136,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="148" spans="1:6">
-      <c r="A148" s="15" t="n">
+      <c r="A148" s="14" t="n">
         <v>40646971</v>
       </c>
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="13" t="s">
         <v>143</v>
       </c>
       <c r="C148" s="10" t="n">
@@ -4638,10 +4156,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="149" spans="1:6">
-      <c r="A149" s="15" t="n">
+      <c r="A149" s="14" t="n">
         <v>40690752</v>
       </c>
-      <c r="B149" s="14" t="s">
+      <c r="B149" s="13" t="s">
         <v>144</v>
       </c>
       <c r="C149" s="10" t="n">
@@ -4658,10 +4176,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="150" spans="1:6">
-      <c r="A150" s="15" t="n">
+      <c r="A150" s="14" t="n">
         <v>70561696</v>
       </c>
-      <c r="B150" s="14" t="s">
+      <c r="B150" s="13" t="s">
         <v>145</v>
       </c>
       <c r="C150" s="10" t="n">
@@ -4678,10 +4196,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="151" spans="1:6">
-      <c r="A151" s="15" t="n">
+      <c r="A151" s="14" t="n">
         <v>71432278</v>
       </c>
-      <c r="B151" s="14" t="s">
+      <c r="B151" s="13" t="s">
         <v>146</v>
       </c>
       <c r="C151" s="10" t="n">
@@ -4698,10 +4216,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="152" spans="1:6">
-      <c r="A152" s="15" t="n">
+      <c r="A152" s="14" t="n">
         <v>40087057</v>
       </c>
-      <c r="B152" s="14" t="s">
+      <c r="B152" s="13" t="s">
         <v>147</v>
       </c>
       <c r="C152" s="10" t="n">
@@ -4718,10 +4236,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="153" spans="1:6">
-      <c r="A153" s="15" t="n">
+      <c r="A153" s="14" t="n">
         <v>70341595</v>
       </c>
-      <c r="B153" s="14" t="s">
+      <c r="B153" s="13" t="s">
         <v>148</v>
       </c>
       <c r="C153" s="10" t="n">
@@ -4738,10 +4256,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="154" spans="1:6">
-      <c r="A154" s="15" t="n">
+      <c r="A154" s="14" t="n">
         <v>70551529</v>
       </c>
-      <c r="B154" s="14" t="s">
+      <c r="B154" s="13" t="s">
         <v>149</v>
       </c>
       <c r="C154" s="10" t="n">
@@ -4758,10 +4276,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="155" spans="1:6">
-      <c r="A155" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="B155" s="14" t="s">
+      <c r="A155" s="14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B155" s="13" t="s">
         <v>150</v>
       </c>
       <c r="C155" s="10" t="n">
@@ -4778,10 +4296,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="156" spans="1:6">
-      <c r="A156" s="15" t="n">
+      <c r="A156" s="14" t="n">
         <v>40690936</v>
       </c>
-      <c r="B156" s="14" t="s">
+      <c r="B156" s="13" t="s">
         <v>151</v>
       </c>
       <c r="C156" s="10" t="n">
@@ -4798,10 +4316,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="157" spans="1:6">
-      <c r="A157" s="15" t="n">
+      <c r="A157" s="14" t="n">
         <v>70431814</v>
       </c>
-      <c r="B157" s="14" t="s">
+      <c r="B157" s="13" t="s">
         <v>152</v>
       </c>
       <c r="C157" s="10" t="n">
@@ -4818,10 +4336,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="158" spans="1:6">
-      <c r="A158" s="15" t="n">
+      <c r="A158" s="14" t="n">
         <v>71432285</v>
       </c>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="13" t="s">
         <v>153</v>
       </c>
       <c r="C158" s="10" t="n">
@@ -4838,10 +4356,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="159" spans="1:6">
-      <c r="A159" s="15" t="n">
+      <c r="A159" s="14" t="n">
         <v>71033970</v>
       </c>
-      <c r="B159" s="14" t="s">
+      <c r="B159" s="13" t="s">
         <v>154</v>
       </c>
       <c r="C159" s="10" t="n">
@@ -4858,10 +4376,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="160" spans="1:6">
-      <c r="A160" s="15" t="n">
+      <c r="A160" s="14" t="n">
         <v>71346889</v>
       </c>
-      <c r="B160" s="14" t="s">
+      <c r="B160" s="13" t="s">
         <v>155</v>
       </c>
       <c r="C160" s="10" t="n">
@@ -4878,10 +4396,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="161" spans="1:6">
-      <c r="A161" s="15" t="n">
+      <c r="A161" s="14" t="n">
         <v>71034120</v>
       </c>
-      <c r="B161" s="14" t="s">
+      <c r="B161" s="13" t="s">
         <v>156</v>
       </c>
       <c r="C161" s="10" t="n">
@@ -4898,10 +4416,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="162" spans="1:6">
-      <c r="A162" s="15" t="n">
+      <c r="A162" s="14" t="n">
         <v>71039828</v>
       </c>
-      <c r="B162" s="14" t="s">
+      <c r="B162" s="13" t="s">
         <v>157</v>
       </c>
       <c r="C162" s="10" t="n">
@@ -4918,10 +4436,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="163" spans="1:6">
-      <c r="A163" s="15" t="n">
+      <c r="A163" s="14" t="n">
         <v>70341564</v>
       </c>
-      <c r="B163" s="14" t="s">
+      <c r="B163" s="13" t="s">
         <v>158</v>
       </c>
       <c r="C163" s="10" t="n">
@@ -4938,10 +4456,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="164" spans="1:6">
-      <c r="A164" s="15" t="n">
+      <c r="A164" s="14" t="n">
         <v>70561634</v>
       </c>
-      <c r="B164" s="14" t="s">
+      <c r="B164" s="13" t="s">
         <v>159</v>
       </c>
       <c r="C164" s="10" t="n">
@@ -4958,10 +4476,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="165" spans="1:6">
-      <c r="A165" s="15" t="n">
+      <c r="A165" s="14" t="n">
         <v>40787971</v>
       </c>
-      <c r="B165" s="14" t="s">
+      <c r="B165" s="13" t="s">
         <v>160</v>
       </c>
       <c r="C165" s="10" t="n">
@@ -4978,10 +4496,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="166" spans="1:6">
-      <c r="A166" s="15" t="n">
+      <c r="A166" s="14" t="n">
         <v>40556263</v>
       </c>
-      <c r="B166" s="14" t="s">
+      <c r="B166" s="13" t="s">
         <v>161</v>
       </c>
       <c r="C166" s="10" t="n">
@@ -4998,10 +4516,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="167" spans="1:6">
-      <c r="A167" s="15" t="n">
+      <c r="A167" s="14" t="n">
         <v>21250313</v>
       </c>
-      <c r="B167" s="14" t="s">
+      <c r="B167" s="13" t="s">
         <v>162</v>
       </c>
       <c r="C167" s="10" t="n">
@@ -5018,10 +4536,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="168" spans="1:6">
-      <c r="A168" s="15" t="n">
+      <c r="A168" s="14" t="n">
         <v>21250290</v>
       </c>
-      <c r="B168" s="14" t="s">
+      <c r="B168" s="13" t="s">
         <v>163</v>
       </c>
       <c r="C168" s="10" t="n">
@@ -5038,10 +4556,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="169" spans="1:6">
-      <c r="A169" s="15" t="n">
+      <c r="A169" s="14" t="n">
         <v>21250283</v>
       </c>
-      <c r="B169" s="14" t="s">
+      <c r="B169" s="13" t="s">
         <v>164</v>
       </c>
       <c r="C169" s="10" t="n">
@@ -5058,10 +4576,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="170" spans="1:6">
-      <c r="A170" s="15" t="n">
+      <c r="A170" s="14" t="n">
         <v>21250351</v>
       </c>
-      <c r="B170" s="14" t="s">
+      <c r="B170" s="13" t="s">
         <v>165</v>
       </c>
       <c r="C170" s="10" t="n">
@@ -5078,10 +4596,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="171" spans="1:6">
-      <c r="A171" s="15" t="n">
+      <c r="A171" s="14" t="n">
         <v>21250306</v>
       </c>
-      <c r="B171" s="14" t="s">
+      <c r="B171" s="13" t="s">
         <v>166</v>
       </c>
       <c r="C171" s="10" t="n">
@@ -5098,10 +4616,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="172" spans="1:6">
-      <c r="A172" s="15" t="n">
+      <c r="A172" s="14" t="n">
         <v>21250337</v>
       </c>
-      <c r="B172" s="14" t="s">
+      <c r="B172" s="13" t="s">
         <v>167</v>
       </c>
       <c r="C172" s="10" t="n">
@@ -5118,10 +4636,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="173" spans="1:6">
-      <c r="A173" s="15" t="n">
+      <c r="A173" s="14" t="n">
         <v>21250320</v>
       </c>
-      <c r="B173" s="14" t="s">
+      <c r="B173" s="13" t="s">
         <v>168</v>
       </c>
       <c r="C173" s="10" t="n">
@@ -5138,10 +4656,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="174" spans="1:6">
-      <c r="A174" s="15" t="n">
+      <c r="A174" s="14" t="n">
         <v>21250344</v>
       </c>
-      <c r="B174" s="14" t="s">
+      <c r="B174" s="13" t="s">
         <v>169</v>
       </c>
       <c r="C174" s="10" t="n">
@@ -5158,10 +4676,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="175" spans="1:6">
-      <c r="A175" s="15" t="n">
+      <c r="A175" s="14" t="n">
         <v>95437109</v>
       </c>
-      <c r="B175" s="14" t="s">
+      <c r="B175" s="13" t="s">
         <v>170</v>
       </c>
       <c r="C175" s="10" t="n">
@@ -5178,10 +4696,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="176" spans="1:6">
-      <c r="A176" s="15" t="n">
+      <c r="A176" s="14" t="n">
         <v>95437123</v>
       </c>
-      <c r="B176" s="14" t="s">
+      <c r="B176" s="13" t="s">
         <v>171</v>
       </c>
       <c r="C176" s="10" t="n">
@@ -5198,10 +4716,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="177" spans="1:6">
-      <c r="A177" s="15" t="n">
+      <c r="A177" s="14" t="n">
         <v>95437154</v>
       </c>
-      <c r="B177" s="14" t="s">
+      <c r="B177" s="13" t="s">
         <v>172</v>
       </c>
       <c r="C177" s="10" t="n">
@@ -5218,10 +4736,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="178" spans="1:6">
-      <c r="A178" s="15" t="n">
+      <c r="A178" s="14" t="n">
         <v>95437161</v>
       </c>
-      <c r="B178" s="14" t="s">
+      <c r="B178" s="13" t="s">
         <v>173</v>
       </c>
       <c r="C178" s="10" t="n">
@@ -5238,10 +4756,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="179" spans="1:6">
-      <c r="A179" s="15" t="n">
+      <c r="A179" s="14" t="n">
         <v>95437178</v>
       </c>
-      <c r="B179" s="14" t="s">
+      <c r="B179" s="13" t="s">
         <v>174</v>
       </c>
       <c r="C179" s="10" t="n">
@@ -5258,10 +4776,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="180" spans="1:6">
-      <c r="A180" s="15" t="n">
+      <c r="A180" s="14" t="n">
         <v>95437147</v>
       </c>
-      <c r="B180" s="14" t="s">
+      <c r="B180" s="13" t="s">
         <v>175</v>
       </c>
       <c r="C180" s="10" t="n">
@@ -5278,10 +4796,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="181" spans="1:6">
-      <c r="A181" s="15" t="n">
+      <c r="A181" s="14" t="n">
         <v>95437185</v>
       </c>
-      <c r="B181" s="14" t="s">
+      <c r="B181" s="13" t="s">
         <v>176</v>
       </c>
       <c r="C181" s="10" t="n">
@@ -5298,10 +4816,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="182" spans="1:6">
-      <c r="A182" s="15" t="n">
+      <c r="A182" s="14" t="n">
         <v>49074541</v>
       </c>
-      <c r="B182" s="14" t="s">
+      <c r="B182" s="13" t="s">
         <v>177</v>
       </c>
       <c r="C182" s="10" t="n">
@@ -5318,10 +4836,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="183" spans="1:6">
-      <c r="A183" s="15" t="n">
+      <c r="A183" s="14" t="n">
         <v>49045824</v>
       </c>
-      <c r="B183" s="14" t="s">
+      <c r="B183" s="13" t="s">
         <v>178</v>
       </c>
       <c r="C183" s="10" t="n">
@@ -5338,10 +4856,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="184" spans="1:6">
-      <c r="A184" s="15" t="n">
+      <c r="A184" s="14" t="n">
         <v>49045657</v>
       </c>
-      <c r="B184" s="14" t="s">
+      <c r="B184" s="13" t="s">
         <v>179</v>
       </c>
       <c r="C184" s="10" t="n">
@@ -5358,10 +4876,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="185" spans="1:6">
-      <c r="A185" s="15" t="n">
+      <c r="A185" s="14" t="n">
         <v>49083727</v>
       </c>
-      <c r="B185" s="14" t="s">
+      <c r="B185" s="13" t="s">
         <v>180</v>
       </c>
       <c r="C185" s="10" t="n">
@@ -5378,10 +4896,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="186" spans="1:6">
-      <c r="A186" s="15" t="n">
+      <c r="A186" s="14" t="n">
         <v>49045961</v>
       </c>
-      <c r="B186" s="14" t="s">
+      <c r="B186" s="13" t="s">
         <v>181</v>
       </c>
       <c r="C186" s="10" t="n">
@@ -5398,10 +4916,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="187" spans="1:6">
-      <c r="A187" s="15" t="n">
+      <c r="A187" s="14" t="n">
         <v>49074558</v>
       </c>
-      <c r="B187" s="14" t="s">
+      <c r="B187" s="13" t="s">
         <v>182</v>
       </c>
       <c r="C187" s="10" t="n">
@@ -5418,10 +4936,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="188" spans="1:6">
-      <c r="A188" s="15" t="n">
+      <c r="A188" s="14" t="n">
         <v>49046029</v>
       </c>
-      <c r="B188" s="14" t="s">
+      <c r="B188" s="13" t="s">
         <v>183</v>
       </c>
       <c r="C188" s="10" t="n">
@@ -5438,10 +4956,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="189" spans="1:6">
-      <c r="A189" s="15" t="n">
+      <c r="A189" s="14" t="n">
         <v>49045640</v>
       </c>
-      <c r="B189" s="14" t="s">
+      <c r="B189" s="13" t="s">
         <v>184</v>
       </c>
       <c r="C189" s="10" t="n">
@@ -5458,10 +4976,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="190" spans="1:6">
-      <c r="A190" s="15" t="n">
+      <c r="A190" s="14" t="n">
         <v>95467687</v>
       </c>
-      <c r="B190" s="14" t="s">
+      <c r="B190" s="13" t="s">
         <v>185</v>
       </c>
       <c r="C190" s="10" t="n">
@@ -5478,10 +4996,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="191" spans="1:6">
-      <c r="A191" s="15" t="n">
+      <c r="A191" s="14" t="n">
         <v>95467700</v>
       </c>
-      <c r="B191" s="14" t="s">
+      <c r="B191" s="13" t="s">
         <v>186</v>
       </c>
       <c r="C191" s="10" t="n">
@@ -5498,10 +5016,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="192" spans="1:6">
-      <c r="A192" s="15" t="n">
+      <c r="A192" s="14" t="n">
         <v>95467724</v>
       </c>
-      <c r="B192" s="14" t="s">
+      <c r="B192" s="13" t="s">
         <v>187</v>
       </c>
       <c r="C192" s="10" t="n">
@@ -5518,10 +5036,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="193" spans="1:6">
-      <c r="A193" s="15" t="n">
+      <c r="A193" s="14" t="n">
         <v>49168370</v>
       </c>
-      <c r="B193" s="14" t="s">
+      <c r="B193" s="13" t="s">
         <v>188</v>
       </c>
       <c r="C193" s="10" t="n">
@@ -5538,10 +5056,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="194" spans="1:6">
-      <c r="A194" s="15" t="n">
+      <c r="A194" s="14" t="n">
         <v>49168431</v>
       </c>
-      <c r="B194" s="14" t="s">
+      <c r="B194" s="13" t="s">
         <v>189</v>
       </c>
       <c r="C194" s="10" t="n">
@@ -5558,10 +5076,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="195" spans="1:6">
-      <c r="A195" s="15" t="n">
+      <c r="A195" s="14" t="n">
         <v>49168448</v>
       </c>
-      <c r="B195" s="14" t="s">
+      <c r="B195" s="13" t="s">
         <v>190</v>
       </c>
       <c r="C195" s="10" t="n">
@@ -5578,10 +5096,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="196" spans="1:6">
-      <c r="A196" s="15" t="n">
+      <c r="A196" s="14" t="n">
         <v>49168479</v>
       </c>
-      <c r="B196" s="14" t="s">
+      <c r="B196" s="13" t="s">
         <v>191</v>
       </c>
       <c r="C196" s="10" t="n">
@@ -5598,10 +5116,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="197" spans="1:6">
-      <c r="A197" s="15" t="n">
+      <c r="A197" s="14" t="n">
         <v>49168530</v>
       </c>
-      <c r="B197" s="14" t="s">
+      <c r="B197" s="13" t="s">
         <v>192</v>
       </c>
       <c r="C197" s="10" t="n">
@@ -5618,10 +5136,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="198" spans="1:6">
-      <c r="A198" s="15" t="n">
+      <c r="A198" s="14" t="n">
         <v>49168547</v>
       </c>
-      <c r="B198" s="14" t="s">
+      <c r="B198" s="13" t="s">
         <v>193</v>
       </c>
       <c r="C198" s="10" t="n">
@@ -5638,10 +5156,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="199" spans="1:6">
-      <c r="A199" s="15" t="n">
+      <c r="A199" s="14" t="n">
         <v>49168554</v>
       </c>
-      <c r="B199" s="14" t="s">
+      <c r="B199" s="13" t="s">
         <v>194</v>
       </c>
       <c r="C199" s="10" t="n">
@@ -5658,10 +5176,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="200" spans="1:6">
-      <c r="A200" s="15" t="n">
+      <c r="A200" s="14" t="n">
         <v>49168561</v>
       </c>
-      <c r="B200" s="14" t="s">
+      <c r="B200" s="13" t="s">
         <v>195</v>
       </c>
       <c r="C200" s="10" t="n">
@@ -5678,10 +5196,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="201" spans="1:6">
-      <c r="A201" s="15" t="n">
+      <c r="A201" s="14" t="n">
         <v>49168578</v>
       </c>
-      <c r="B201" s="14" t="s">
+      <c r="B201" s="13" t="s">
         <v>196</v>
       </c>
       <c r="C201" s="10" t="n">
@@ -5698,10 +5216,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="202" spans="1:6">
-      <c r="A202" s="15" t="n">
+      <c r="A202" s="14" t="n">
         <v>49168585</v>
       </c>
-      <c r="B202" s="14" t="s">
+      <c r="B202" s="13" t="s">
         <v>197</v>
       </c>
       <c r="C202" s="10" t="n">
@@ -5718,10 +5236,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="203" spans="1:6">
-      <c r="A203" s="15" t="n">
+      <c r="A203" s="14" t="n">
         <v>49168622</v>
       </c>
-      <c r="B203" s="14" t="s">
+      <c r="B203" s="13" t="s">
         <v>198</v>
       </c>
       <c r="C203" s="10" t="n">
@@ -5738,10 +5256,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="204" spans="1:6">
-      <c r="A204" s="15" t="n">
+      <c r="A204" s="14" t="n">
         <v>49215562</v>
       </c>
-      <c r="B204" s="14" t="s">
+      <c r="B204" s="13" t="s">
         <v>199</v>
       </c>
       <c r="C204" s="10" t="n">
@@ -5758,10 +5276,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="205" spans="1:6">
-      <c r="A205" s="15" t="n">
+      <c r="A205" s="14" t="n">
         <v>95416159</v>
       </c>
-      <c r="B205" s="14" t="s">
+      <c r="B205" s="13" t="s">
         <v>200</v>
       </c>
       <c r="C205" s="10" t="n">
@@ -5778,10 +5296,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="206" spans="1:6">
-      <c r="A206" s="15" t="n">
+      <c r="A206" s="14" t="n">
         <v>95416166</v>
       </c>
-      <c r="B206" s="14" t="s">
+      <c r="B206" s="13" t="s">
         <v>201</v>
       </c>
       <c r="C206" s="10" t="n">
@@ -5798,10 +5316,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="207" spans="1:6">
-      <c r="A207" s="15" t="n">
+      <c r="A207" s="14" t="n">
         <v>95416173</v>
       </c>
-      <c r="B207" s="14" t="s">
+      <c r="B207" s="13" t="s">
         <v>202</v>
       </c>
       <c r="C207" s="10" t="n">
@@ -5818,10 +5336,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="208" spans="1:6">
-      <c r="A208" s="15" t="n">
+      <c r="A208" s="14" t="n">
         <v>95416197</v>
       </c>
-      <c r="B208" s="14" t="s">
+      <c r="B208" s="13" t="s">
         <v>203</v>
       </c>
       <c r="C208" s="10" t="n">
@@ -5838,10 +5356,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="209" spans="1:6">
-      <c r="A209" s="15" t="n">
+      <c r="A209" s="14" t="n">
         <v>95416227</v>
       </c>
-      <c r="B209" s="14" t="s">
+      <c r="B209" s="13" t="s">
         <v>204</v>
       </c>
       <c r="C209" s="10" t="n">
@@ -5858,10 +5376,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="210" spans="1:6">
-      <c r="A210" s="15" t="n">
+      <c r="A210" s="14" t="n">
         <v>95445609</v>
       </c>
-      <c r="B210" s="14" t="s">
+      <c r="B210" s="13" t="s">
         <v>205</v>
       </c>
       <c r="C210" s="10" t="n">
@@ -5878,10 +5396,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="211" spans="1:6">
-      <c r="A211" s="15" t="n">
+      <c r="A211" s="14" t="n">
         <v>95445623</v>
       </c>
-      <c r="B211" s="14" t="s">
+      <c r="B211" s="13" t="s">
         <v>206</v>
       </c>
       <c r="C211" s="10" t="n">
@@ -5898,10 +5416,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="212" spans="1:6">
-      <c r="A212" s="15" t="n">
+      <c r="A212" s="14" t="n">
         <v>95445630</v>
       </c>
-      <c r="B212" s="14" t="s">
+      <c r="B212" s="13" t="s">
         <v>207</v>
       </c>
       <c r="C212" s="10" t="n">
@@ -5918,10 +5436,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="213" spans="1:6">
-      <c r="A213" s="15" t="n">
+      <c r="A213" s="14" t="n">
         <v>95445654</v>
       </c>
-      <c r="B213" s="14" t="s">
+      <c r="B213" s="13" t="s">
         <v>208</v>
       </c>
       <c r="C213" s="10" t="n">
@@ -5938,10 +5456,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="214" spans="1:6">
-      <c r="A214" s="15" t="n">
+      <c r="A214" s="14" t="n">
         <v>49314432</v>
       </c>
-      <c r="B214" s="14" t="s">
+      <c r="B214" s="13" t="s">
         <v>209</v>
       </c>
       <c r="C214" s="10" t="n">
@@ -5958,10 +5476,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="215" spans="1:6">
-      <c r="A215" s="15" t="n">
+      <c r="A215" s="14" t="n">
         <v>49314395</v>
       </c>
-      <c r="B215" s="14" t="s">
+      <c r="B215" s="13" t="s">
         <v>210</v>
       </c>
       <c r="C215" s="10" t="n">
@@ -5978,10 +5496,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="216" spans="1:6">
-      <c r="A216" s="15" t="n">
+      <c r="A216" s="14" t="n">
         <v>49314388</v>
       </c>
-      <c r="B216" s="14" t="s">
+      <c r="B216" s="13" t="s">
         <v>211</v>
       </c>
       <c r="C216" s="10" t="n">
@@ -5998,10 +5516,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="217" spans="1:6">
-      <c r="A217" s="15" t="n">
+      <c r="A217" s="14" t="n">
         <v>49314364</v>
       </c>
-      <c r="B217" s="14" t="s">
+      <c r="B217" s="13" t="s">
         <v>212</v>
       </c>
       <c r="C217" s="10" t="n">
@@ -6018,10 +5536,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="218" spans="1:6">
-      <c r="A218" s="15" t="n">
+      <c r="A218" s="14" t="n">
         <v>49314463</v>
       </c>
-      <c r="B218" s="14" t="s">
+      <c r="B218" s="13" t="s">
         <v>213</v>
       </c>
       <c r="C218" s="10" t="n">
@@ -6038,10 +5556,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="219" spans="1:6">
-      <c r="A219" s="15" t="n">
+      <c r="A219" s="14" t="n">
         <v>49314449</v>
       </c>
-      <c r="B219" s="14" t="s">
+      <c r="B219" s="13" t="s">
         <v>214</v>
       </c>
       <c r="C219" s="10" t="n">
@@ -6058,10 +5576,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="220" spans="1:6">
-      <c r="A220" s="15" t="n">
+      <c r="A220" s="14" t="n">
         <v>49299081</v>
       </c>
-      <c r="B220" s="14" t="s">
+      <c r="B220" s="13" t="s">
         <v>215</v>
       </c>
       <c r="C220" s="10" t="n">
@@ -6078,10 +5596,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="221" spans="1:6">
-      <c r="A221" s="15" t="n">
+      <c r="A221" s="14" t="n">
         <v>49299074</v>
       </c>
-      <c r="B221" s="14" t="s">
+      <c r="B221" s="13" t="s">
         <v>216</v>
       </c>
       <c r="C221" s="10" t="n">
@@ -6098,10 +5616,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="222" spans="1:6">
-      <c r="A222" s="15" t="n">
+      <c r="A222" s="14" t="n">
         <v>21260589</v>
       </c>
-      <c r="B222" s="14" t="s">
+      <c r="B222" s="13" t="s">
         <v>217</v>
       </c>
       <c r="C222" s="10" t="n">
@@ -6118,10 +5636,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="223" spans="1:6">
-      <c r="A223" s="15" t="n">
+      <c r="A223" s="14" t="n">
         <v>21260558</v>
       </c>
-      <c r="B223" s="14" t="s">
+      <c r="B223" s="13" t="s">
         <v>218</v>
       </c>
       <c r="C223" s="10" t="n">
@@ -6138,10 +5656,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="224" spans="1:6">
-      <c r="A224" s="15" t="n">
+      <c r="A224" s="14" t="n">
         <v>18223759</v>
       </c>
-      <c r="B224" s="14" t="s">
+      <c r="B224" s="13" t="s">
         <v>219</v>
       </c>
       <c r="C224" s="10" t="n">
@@ -6158,10 +5676,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="225" spans="1:6">
-      <c r="A225" s="15" t="n">
+      <c r="A225" s="14" t="n">
         <v>49294055</v>
       </c>
-      <c r="B225" s="14" t="s">
+      <c r="B225" s="13" t="s">
         <v>220</v>
       </c>
       <c r="C225" s="10" t="n">
@@ -6178,10 +5696,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="226" spans="1:6">
-      <c r="A226" s="15" t="n">
+      <c r="A226" s="14" t="n">
         <v>49313039</v>
       </c>
-      <c r="B226" s="14" t="s">
+      <c r="B226" s="13" t="s">
         <v>221</v>
       </c>
       <c r="C226" s="10" t="n">
@@ -6198,10 +5716,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="227" spans="1:6">
-      <c r="A227" s="15" t="n">
+      <c r="A227" s="14" t="n">
         <v>37039448</v>
       </c>
-      <c r="B227" s="14" t="s">
+      <c r="B227" s="13" t="s">
         <v>222</v>
       </c>
       <c r="C227" s="10" t="n">
@@ -6218,10 +5736,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="228" spans="1:6">
-      <c r="A228" s="15" t="n">
+      <c r="A228" s="14" t="n">
         <v>44214161</v>
       </c>
-      <c r="B228" s="14" t="s">
+      <c r="B228" s="13" t="s">
         <v>223</v>
       </c>
       <c r="C228" s="10" t="n">
@@ -6238,10 +5756,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="229" spans="1:6">
-      <c r="A229" s="15" t="n">
+      <c r="A229" s="14" t="n">
         <v>44214154</v>
       </c>
-      <c r="B229" s="14" t="s">
+      <c r="B229" s="13" t="s">
         <v>224</v>
       </c>
       <c r="C229" s="10" t="n">
@@ -6258,10 +5776,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="230" spans="1:6">
-      <c r="A230" s="15" t="n">
+      <c r="A230" s="14" t="n">
         <v>95356691</v>
       </c>
-      <c r="B230" s="14" t="s">
+      <c r="B230" s="13" t="s">
         <v>225</v>
       </c>
       <c r="C230" s="10" t="n">
@@ -6278,10 +5796,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="231" spans="1:6">
-      <c r="A231" s="15" t="n">
+      <c r="A231" s="14" t="n">
         <v>95356707</v>
       </c>
-      <c r="B231" s="14" t="s">
+      <c r="B231" s="13" t="s">
         <v>226</v>
       </c>
       <c r="C231" s="10" t="n">
@@ -6298,10 +5816,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="232" spans="1:6">
-      <c r="A232" s="15" t="n">
+      <c r="A232" s="14" t="n">
         <v>95356714</v>
       </c>
-      <c r="B232" s="14" t="s">
+      <c r="B232" s="13" t="s">
         <v>227</v>
       </c>
       <c r="C232" s="10" t="n">
@@ -6318,10 +5836,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="233" spans="1:6">
-      <c r="A233" s="15" t="n">
+      <c r="A233" s="14" t="n">
         <v>95356721</v>
       </c>
-      <c r="B233" s="14" t="s">
+      <c r="B233" s="13" t="s">
         <v>228</v>
       </c>
       <c r="C233" s="10" t="n">
@@ -6338,10 +5856,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="234" spans="1:6">
-      <c r="A234" s="15" t="n">
+      <c r="A234" s="14" t="n">
         <v>95307259</v>
       </c>
-      <c r="B234" s="14" t="s">
+      <c r="B234" s="13" t="s">
         <v>229</v>
       </c>
       <c r="C234" s="10" t="n">
@@ -6358,10 +5876,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="235" spans="1:6">
-      <c r="A235" s="15" t="n">
+      <c r="A235" s="14" t="n">
         <v>95307112</v>
       </c>
-      <c r="B235" s="14" t="s">
+      <c r="B235" s="13" t="s">
         <v>230</v>
       </c>
       <c r="C235" s="10" t="n">
@@ -6378,10 +5896,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="236" spans="1:6">
-      <c r="A236" s="15" t="n">
+      <c r="A236" s="14" t="n">
         <v>44211047</v>
       </c>
-      <c r="B236" s="14" t="s">
+      <c r="B236" s="13" t="s">
         <v>231</v>
       </c>
       <c r="C236" s="10" t="n">
@@ -6398,10 +5916,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="237" spans="1:6">
-      <c r="A237" s="15" t="n">
+      <c r="A237" s="14" t="n">
         <v>44211030</v>
       </c>
-      <c r="B237" s="14" t="s">
+      <c r="B237" s="13" t="s">
         <v>232</v>
       </c>
       <c r="C237" s="10" t="n">
@@ -6418,10 +5936,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="238" spans="1:6">
-      <c r="A238" s="15" t="n">
+      <c r="A238" s="14" t="n">
         <v>49187722</v>
       </c>
-      <c r="B238" s="14" t="s">
+      <c r="B238" s="13" t="s">
         <v>233</v>
       </c>
       <c r="C238" s="10" t="n">
@@ -6438,10 +5956,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="239" spans="1:6">
-      <c r="A239" s="15" t="n">
+      <c r="A239" s="14" t="n">
         <v>4017827</v>
       </c>
-      <c r="B239" s="14" t="s">
+      <c r="B239" s="13" t="s">
         <v>234</v>
       </c>
       <c r="C239" s="10" t="n">
@@ -6458,10 +5976,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="240" spans="1:6">
-      <c r="A240" s="15" t="n">
+      <c r="A240" s="14" t="n">
         <v>18269771</v>
       </c>
-      <c r="B240" s="14" t="s">
+      <c r="B240" s="13" t="s">
         <v>235</v>
       </c>
       <c r="C240" s="10" t="n">
@@ -6478,10 +5996,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="241" spans="1:6">
-      <c r="A241" s="15" t="n">
+      <c r="A241" s="14" t="n">
         <v>95356103</v>
       </c>
-      <c r="B241" s="14" t="s">
+      <c r="B241" s="13" t="s">
         <v>236</v>
       </c>
       <c r="C241" s="10" t="n">
@@ -6498,10 +6016,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="242" spans="1:6">
-      <c r="A242" s="15" t="n">
+      <c r="A242" s="14" t="n">
         <v>22895431</v>
       </c>
-      <c r="B242" s="14" t="s">
+      <c r="B242" s="13" t="s">
         <v>237</v>
       </c>
       <c r="C242" s="10" t="n">
@@ -6518,10 +6036,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="243" spans="1:6">
-      <c r="A243" s="15" t="n">
+      <c r="A243" s="14" t="n">
         <v>22895448</v>
       </c>
-      <c r="B243" s="14" t="s">
+      <c r="B243" s="13" t="s">
         <v>238</v>
       </c>
       <c r="C243" s="10" t="n">
@@ -6538,10 +6056,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="244" spans="1:6">
-      <c r="A244" s="15" t="n">
+      <c r="A244" s="14" t="n">
         <v>18203881</v>
       </c>
-      <c r="B244" s="14" t="s">
+      <c r="B244" s="13" t="s">
         <v>239</v>
       </c>
       <c r="C244" s="10" t="n">
@@ -6558,10 +6076,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="245" spans="1:6">
-      <c r="A245" s="15" t="n">
+      <c r="A245" s="14" t="n">
         <v>18245652</v>
       </c>
-      <c r="B245" s="14" t="s">
+      <c r="B245" s="13" t="s">
         <v>240</v>
       </c>
       <c r="C245" s="10" t="n">
@@ -6578,10 +6096,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="246" spans="1:6">
-      <c r="A246" s="15" t="n">
+      <c r="A246" s="14" t="n">
         <v>18271910</v>
       </c>
-      <c r="B246" s="14" t="s">
+      <c r="B246" s="13" t="s">
         <v>241</v>
       </c>
       <c r="C246" s="10" t="n">
@@ -6598,10 +6116,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="247" spans="1:6">
-      <c r="A247" s="15" t="n">
+      <c r="A247" s="14" t="n">
         <v>80233213</v>
       </c>
-      <c r="B247" s="14" t="s">
+      <c r="B247" s="13" t="s">
         <v>242</v>
       </c>
       <c r="C247" s="10" t="n">
@@ -6618,10 +6136,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="248" spans="1:6">
-      <c r="A248" s="15" t="n">
+      <c r="A248" s="14" t="n">
         <v>4031137</v>
       </c>
-      <c r="B248" s="14" t="s">
+      <c r="B248" s="13" t="s">
         <v>243</v>
       </c>
       <c r="C248" s="10" t="n">
@@ -6638,10 +6156,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="249" spans="1:6">
-      <c r="A249" s="15" t="n">
+      <c r="A249" s="14" t="n">
         <v>4042171</v>
       </c>
-      <c r="B249" s="14" t="s">
+      <c r="B249" s="13" t="s">
         <v>244</v>
       </c>
       <c r="C249" s="10" t="n">
@@ -6658,10 +6176,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="250" spans="1:6">
-      <c r="A250" s="15" t="n">
+      <c r="A250" s="14" t="n">
         <v>20009345</v>
       </c>
-      <c r="B250" s="14" t="s">
+      <c r="B250" s="13" t="s">
         <v>245</v>
       </c>
       <c r="C250" s="10" t="n">
@@ -6678,10 +6196,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="251" spans="1:6">
-      <c r="A251" s="15" t="n">
+      <c r="A251" s="14" t="n">
         <v>18223926</v>
       </c>
-      <c r="B251" s="14" t="s">
+      <c r="B251" s="13" t="s">
         <v>246</v>
       </c>
       <c r="C251" s="10" t="n">
@@ -6698,10 +6216,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="252" spans="1:6">
-      <c r="A252" s="15" t="n">
+      <c r="A252" s="14" t="n">
         <v>18265490</v>
       </c>
-      <c r="B252" s="14" t="s">
+      <c r="B252" s="13" t="s">
         <v>247</v>
       </c>
       <c r="C252" s="10" t="n">
@@ -6718,10 +6236,10 @@
       </c>
     </row>
     <row customHeight="1" ht="14.4" r="253" spans="1:6">
-      <c r="A253" s="15" t="n">
+      <c r="A253" s="14" t="n">
         <v>34200239</v>
       </c>
-      <c r="B253" s="14" t="s">
+      <c r="B253" s="13" t="s">
         <v>248</v>
       </c>
       <c r="C253" s="10" t="n">

</xml_diff>